<commit_message>
DRP - Last correction
</commit_message>
<xml_diff>
--- a/RGPD/template RGPD registos.xlsx
+++ b/RGPD/template RGPD registos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="153" documentId="13_ncr:1_{956C25C9-4560-4D05-8050-855A188EFC65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{03A2E008-DB21-4133-8C4C-9B4C07BE5558}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{956C25C9-4560-4D05-8050-855A188EFC65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{333D622C-2C82-4F5D-8C72-40663CBE3C50}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1693,25 +1693,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1722,6 +1707,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2468,26 +2468,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="48" t="s">
         <v>246</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="50"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="46"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="11" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="51" t="s">
         <v>238</v>
       </c>
-      <c r="B3" s="48"/>
+      <c r="B3" s="52"/>
       <c r="C3" s="11" t="s">
         <v>397</v>
       </c>
@@ -2531,35 +2531,35 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="46"/>
+      <c r="B8" s="44"/>
       <c r="C8" s="34" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="46"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="35">
         <v>279045668</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="52"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="47"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="49"/>
+      <c r="B11" s="43"/>
       <c r="C11" s="5" t="s">
         <v>402</v>
       </c>
@@ -2603,44 +2603,44 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="43"/>
       <c r="C16" s="36" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="49"/>
+      <c r="B17" s="43"/>
       <c r="C17" s="37">
         <v>920145789</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="48" t="s">
         <v>371</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="45"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="50"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="46"/>
+      <c r="B19" s="44"/>
       <c r="C19" s="11" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="51" t="s">
         <v>238</v>
       </c>
-      <c r="B20" s="48"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="11" t="s">
         <v>408</v>
       </c>
@@ -2684,25 +2684,30 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="46"/>
+      <c r="B25" s="44"/>
       <c r="C25" s="34" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="46"/>
+      <c r="B26" s="44"/>
       <c r="C26" s="35">
         <v>279466554</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A10:C10"/>
@@ -2712,11 +2717,6 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C8" r:id="rId1" xr:uid="{04D58837-3C77-46B1-96CD-90ECA1153F10}"/>
@@ -4649,7 +4649,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4712,11 +4712,11 @@
       <c r="G2" s="66" t="s">
         <v>424</v>
       </c>
-      <c r="H2" s="45"/>
+      <c r="H2" s="50"/>
       <c r="I2" s="66" t="s">
         <v>425</v>
       </c>
-      <c r="J2" s="45"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="57" t="s">
         <v>426</v>
       </c>
@@ -7274,8 +7274,8 @@
       <formula1>"sim, não"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="1.2649999999999999" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="95" orientation="landscape" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>